<commit_message>
docs: Update roadmap with completed tasks (Fourier & Portfolio Avg)
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ROADMAP" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EXPERIMENTS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -35,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,74 +434,144 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>TASK</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>AREA</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DESCRIZIONE DETTAGLIATA</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>STRATEGIA IMPLEMENTAZIONE IA</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>FILE COINVOLTI</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>STATO</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>PRIORITÀ</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>BREAKING (SI/NO)</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>INVARIANTS TOCCATI</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>PIANO APPROVATO (SI/NO)</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>TEST RICHIESTI</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>RISULTATO</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>NOTE</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Technical Implementation</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Files</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Effort</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Breaking Change</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Semantics</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Output Num</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Verification</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>End Date</t>
         </is>
       </c>
     </row>
@@ -555,6 +636,20 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -617,6 +712,20 @@
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -679,87 +788,192 @@
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>DATA</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MODELLO</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>PARAMETRI</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>DATASET</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>METRICA</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>RISULTATO</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>NOTE</t>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Fourier UI Control &amp; Window</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Bassa</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>FFT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>window=Hann, N=256</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>SP500 daily</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>stabilità picchi</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Media Portafoglio Equipesata</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Aggiornato renderPortfolio in app.js per filtrare PnL validi e fare media semplice. Visualizzazione "Media Equipesata".</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>frontend/app.js</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Bassa</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
docs: Correctly update roadmap Excel respecting column structure
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,6 +975,178 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Fourier UI Control &amp; Window</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Bassa</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Media Portafoglio Equipesata</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Refactor calcolo media in app.js. Visualizzazione "Media Equipesata".</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>frontend/app.js</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Bassa</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: Standardize roadmap columns as requested
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,76 +504,6 @@
           <t>NOTE</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Technical Implementation</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Files</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Effort</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Breaking Change</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Semantics</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Output Num</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Verification</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Start Date</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>End Date</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -636,20 +566,6 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -712,20 +628,6 @@
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -788,364 +690,270 @@
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fourier UI Control &amp; Window</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Fourier UI Control &amp; Window</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>Bassa</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Media Portafoglio Equipesata</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Aggiornato renderPortfolio in app.js per filtrare PnL validi e fare media semplice. Visualizzazione "Media Equipesata".</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>frontend/app.js</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Media Portafoglio Equipesata</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Aggiornato renderPortfolio in app.js per filtrare PnL validi e fare media semplice. Visualizzazione "Media Equipesata".</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>frontend/app.js</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Bassa</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Fourier UI Control &amp; Window</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Fourier UI Control &amp; Window</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Bassa</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Media Portafoglio Equipesata</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Refactor calcolo media in app.js. Visualizzazione "Media Equipesata".</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>frontend/app.js</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>DONE</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Manuale</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Media Portafoglio Equipesata</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Refactor calcolo media in app.js. Visualizzazione "Media Equipesata".</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>frontend/app.js</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>Bassa</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix: Portfolio fetching (Batch MultiIndex + NaN handling) & Firebase Auth
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,74 +422,99 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>TASK</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>AREA</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>DESCRIZIONE DETTAGLIATA</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>STRATEGIA IMPLEMENTAZIONE IA</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>FILE COINVOLTI</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>STATO</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>PRIORITÀ</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>BREAKING (SI/NO)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>INVARIANTS TOCCATI</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>PIANO APPROVATO (SI/NO)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>TEST RICHIESTI</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>RISULTATO</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>NOTE</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Notes</t>
         </is>
       </c>
     </row>
@@ -566,6 +579,11 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -628,6 +646,11 @@
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -690,6 +713,11 @@
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -756,6 +784,11 @@
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -822,6 +855,11 @@
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -829,131 +867,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fourier UI Control &amp; Window</t>
+          <t>Fix Portfolio Loading Freeze &amp; Price Data NaNs</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Aggiunto pulsante toggle per nascondere/mostrare Fourier e input numerico per definire la finestra di analisi (default 504 giorni).</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Modificato index.html (input/button), app.js (logica toggle + invio param), main.py (ricezione param), logic.py (uso param in FourierEngine).</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>frontend/app.js, frontend/index.html, backend/main.py, backend/logic.py</t>
-        </is>
-      </c>
+          <t>Backend / Infrastructure</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>DONE</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Media Portafoglio Equipesata</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>UI</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Modifica calcolo media rendimenti portafoglio: ora è una media aritmetica non pesata (Equal Weighted) dei %. Ignora null.</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Refactor calcolo media in app.js. Visualizzazione "Media Equipesata".</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>frontend/app.js</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>DONE</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Alta</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Manuale</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr"/>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Resolved Firebase Auth (JWT) error, fixed yfinance batch fetching for MultiIndex, handled NaN prices for US stocks. 2026-01-30</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Meta: Fix roadmap Excel column structure to standard Italian schema
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,31 +492,6 @@
           <t>NOTE</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Area</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -579,11 +554,6 @@
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -646,11 +616,6 @@
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -713,11 +678,6 @@
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -784,11 +744,6 @@
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -855,11 +810,6 @@
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -898,11 +848,6 @@
           <t>Resolved Firebase Auth (JWT) error, fixed yfinance batch fetching for MultiIndex, handled NaN prices for US stocks. 2026-01-30</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Meta: Update roadmap entry with full implementation details
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -825,9 +825,21 @@
           <t>Backend / Infrastructure</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Risoluzione bug critico su fetch prezzi yfinance. 1) I titoli USA restituivano NaN per la giornata corrente (pre-market/festivi). 2) La logica batch aveva un duplicato e gestiva male il MultiIndex per singoli ticker.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Analisi log, creazione script di riproduzione (verify_nan_issue.py, debug_backend_logic.py), patch logica backend.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>backend/main.py</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>Done</t>
@@ -838,11 +850,31 @@
           <t>Critical</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Data Consistency, Real-time Pricing</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Verifica caricamento Portfolio con mix titoli EU/USA; Verifica fallback.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Prezzi corretti visualizzati in dashboard. Fallback attivo.</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr">
         <is>
           <t>Resolved Firebase Auth (JWT) error, fixed yfinance batch fetching for MultiIndex, handled NaN prices for US stocks. 2026-01-30</t>

</xml_diff>

<commit_message>
Fix: Correct email recommendations (cache invalidation) & disable cache default in UI
</commit_message>
<xml_diff>
--- a/memory/financial_physics_roadmap_template.xlsx
+++ b/memory/financial_physics_roadmap_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -881,6 +881,76 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Fix Email HOLD/SELL Recommendations (Cache Invalidation)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Email Scanner</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bug critico: le raccomandazioni HOLD/SELL nell'email giornaliera erano basate su dati cached obsoleti (TICKER_CACHE). Questo causava 3 errori su 9 posizioni: RACE.MI e MUV2.DE mostravano HOLD invece di SELL (strategie chiuse l'11-12/02), MMM mostrava SELL invece di HOLD (strategia aperta dall'11/02). Secondo bug: ticker del portafoglio non presenti in tickers.js non venivano mai scansionati, risultando sempre in SELL.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1) Creazione test standalone (test_email_standalone.py) con caricamento portfolio da Firebase. 2) Analisi indipendente di tutti i 9 ticker del portafoglio per confermare le discrepanze. 3) Invalidazione mirata della TICKER_CACHE per i soli ticker del portafoglio prima dello scan. 4) Merge automatico dei ticker del portafoglio nella lista di scan.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>backend/scanner.py, test_email_standalone.py</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Data Consistency, Email Accuracy</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>1) test_email_standalone.py - confronto raccomandazioni con email reale. 2) Verifica post-deploy: email delle 16:30 deve riflettere stato reale delle strategie.</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Test standalone conferma: 4 HOLD (ITW, JNJ, TTE.PA, PANW), 2 SELL (RACE.MI, MUV2.DE). Tutte le discrepanze con l'email risolte.</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Deploy ID: PENDING (15/02/2026)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>